<commit_message>
A1_Inputs, A1_Outputs, A2_Extra_Inputs, new versions
</commit_message>
<xml_diff>
--- a/Energia/Model/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/Energia/Model/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucr\Documents\Ecuador\t1_confection_v19\A1_Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucr\Desktop\t1_confection_v24_CC_2070_V3\t1_confection_v24_CC_2070_V2\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D46343-2C9F-489A-9C4B-F2580B101B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00589136-2F22-45DD-85DF-9D334CCA66A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand_Projection" sheetId="1" r:id="rId1"/>
     <sheet name="Demand_Calibration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demand_Projection!$A$1:$BK$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demand_Projection!$A$1:$BK$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -531,43 +531,43 @@
     <t>Population coupling</t>
   </si>
   <si>
+    <t>E5_CONREF</t>
+  </si>
+  <si>
+    <t>Demand Refineries Oil</t>
+  </si>
+  <si>
+    <t>E5_BUN</t>
+  </si>
+  <si>
+    <t>Demand for bunkers all fuels</t>
+  </si>
+  <si>
+    <t>E5_CRUTRNCRU</t>
+  </si>
+  <si>
+    <t>E5_CRUTRNELE</t>
+  </si>
+  <si>
+    <t>E5_CRUTRNLPG</t>
+  </si>
+  <si>
+    <t>E5_CRUTRNGSL</t>
+  </si>
+  <si>
+    <t>Demand Electricity SOTE Crude</t>
+  </si>
+  <si>
+    <t>Demand Crude SOTE Crude</t>
+  </si>
+  <si>
+    <t>Demand LPG SOTE Crude</t>
+  </si>
+  <si>
+    <t>Demand GSL SOTE Crude</t>
+  </si>
+  <si>
     <t>GDP transport coupling</t>
-  </si>
-  <si>
-    <t>E5_CONREF</t>
-  </si>
-  <si>
-    <t>Demand Refineries Oil</t>
-  </si>
-  <si>
-    <t>E5_BUN</t>
-  </si>
-  <si>
-    <t>Demand for bunkers all fuels</t>
-  </si>
-  <si>
-    <t>E5_CRUTRNCRU</t>
-  </si>
-  <si>
-    <t>E5_CRUTRNELE</t>
-  </si>
-  <si>
-    <t>E5_CRUTRNLPG</t>
-  </si>
-  <si>
-    <t>E5_CRUTRNGSL</t>
-  </si>
-  <si>
-    <t>Demand Electricity SOTE Crude</t>
-  </si>
-  <si>
-    <t>Demand Crude SOTE Crude</t>
-  </si>
-  <si>
-    <t>Demand LPG SOTE Crude</t>
-  </si>
-  <si>
-    <t>Demand GSL SOTE Crude</t>
   </si>
 </sst>
 </file>
@@ -797,9 +797,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -837,9 +837,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,26 +872,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -924,26 +907,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1119,28 +1085,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH35" sqref="AH35"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O45" sqref="O45:BK45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="21" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="21" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="21" customWidth="1"/>
-    <col min="11" max="63" width="12.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="64" max="16384" width="9.109375" style="21"/>
+    <col min="1" max="1" width="13.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="21" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="21" customWidth="1"/>
+    <col min="11" max="19" width="12.42578125" style="21" customWidth="1"/>
+    <col min="20" max="63" width="12.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="64" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1298,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1386,7 @@
       <c r="BJ2" s="24"/>
       <c r="BK2" s="24"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>101</v>
       </c>
@@ -1505,7 +1472,7 @@
       <c r="BJ3" s="24"/>
       <c r="BK3" s="24"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>101</v>
       </c>
@@ -1591,7 +1558,7 @@
       <c r="BJ4" s="24"/>
       <c r="BK4" s="24"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>101</v>
       </c>
@@ -1677,7 +1644,7 @@
       <c r="BJ5" s="24"/>
       <c r="BK5" s="24"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>101</v>
       </c>
@@ -1762,7 +1729,7 @@
       <c r="BJ6" s="30"/>
       <c r="BK6" s="30"/>
     </row>
-    <row r="7" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1817,7 @@
       <c r="BJ7" s="24"/>
       <c r="BK7" s="24"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>101</v>
       </c>
@@ -1936,7 +1903,7 @@
       <c r="BJ8" s="24"/>
       <c r="BK8" s="24"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>101</v>
       </c>
@@ -2022,7 +1989,7 @@
       <c r="BJ9" s="24"/>
       <c r="BK9" s="24"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>101</v>
       </c>
@@ -2108,7 +2075,7 @@
       <c r="BJ10" s="24"/>
       <c r="BK10" s="24"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>101</v>
       </c>
@@ -2194,7 +2161,7 @@
       <c r="BJ11" s="24"/>
       <c r="BK11" s="24"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>10</v>
       </c>
@@ -2214,7 +2181,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>144</v>
@@ -2226,7 +2193,6 @@
         <v>145</v>
       </c>
       <c r="K12" s="24">
-        <f>(D13*E13*F13 + D14*E14*F14)/1000000000 +K15</f>
         <v>58.961280528000003</v>
       </c>
       <c r="L12" s="24"/>
@@ -2282,7 +2248,7 @@
       <c r="BJ12" s="24"/>
       <c r="BK12" s="24"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>101</v>
       </c>
@@ -2368,7 +2334,7 @@
       <c r="BJ13" s="24"/>
       <c r="BK13" s="24"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>101</v>
       </c>
@@ -2454,7 +2420,7 @@
       <c r="BJ14" s="24"/>
       <c r="BK14" s="24"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>101</v>
       </c>
@@ -2539,7 +2505,7 @@
       <c r="BJ15" s="30"/>
       <c r="BK15" s="30"/>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2525,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>144</v>
@@ -2571,8 +2537,7 @@
         <v>145</v>
       </c>
       <c r="K16" s="24">
-        <f>+D17*E17*F17/1000000000</f>
-        <v>13.754801860799999</v>
+        <v>13.754801860799899</v>
       </c>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
@@ -2627,7 +2592,7 @@
       <c r="BJ16" s="24"/>
       <c r="BK16" s="24"/>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>101</v>
       </c>
@@ -2658,7 +2623,7 @@
       </c>
       <c r="K17" s="24">
         <f>(D17*E17*F17/1000000000)/K16</f>
-        <v>1</v>
+        <v>1.0000000000000073</v>
       </c>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
@@ -2713,7 +2678,7 @@
       <c r="BJ17" s="24"/>
       <c r="BK17" s="24"/>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2698,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>144</v>
@@ -2745,8 +2710,7 @@
         <v>145</v>
       </c>
       <c r="K18" s="24">
-        <f>+D19*E19*F19/1000000000</f>
-        <v>7.1552464108999994</v>
+        <v>7.1552464108999896</v>
       </c>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
@@ -2801,7 +2765,7 @@
       <c r="BJ18" s="24"/>
       <c r="BK18" s="24"/>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>101</v>
       </c>
@@ -2832,7 +2796,7 @@
       </c>
       <c r="K19" s="24">
         <f>(D19*E19*F19/1000000000)/K18</f>
-        <v>1</v>
+        <v>1.0000000000000013</v>
       </c>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
@@ -2887,7 +2851,7 @@
       <c r="BJ19" s="24"/>
       <c r="BK19" s="24"/>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>10</v>
       </c>
@@ -2972,7 +2936,7 @@
       <c r="BJ20" s="24"/>
       <c r="BK20" s="24"/>
     </row>
-    <row r="21" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>10</v>
       </c>
@@ -3163,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>10</v>
       </c>
@@ -3207,7 +3171,7 @@
         <v>2.3650680736738634</v>
       </c>
       <c r="O22" s="22">
-        <v>3.1</v>
+        <v>4.3396384764364102</v>
       </c>
       <c r="P22" s="22">
         <v>3.46</v>
@@ -3354,7 +3318,7 @@
         <v>6.7550391573737691</v>
       </c>
     </row>
-    <row r="23" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>10</v>
       </c>
@@ -3386,166 +3350,166 @@
         <v>14</v>
       </c>
       <c r="K23" s="18">
-        <v>0.18987436107420722</v>
+        <v>4.7630758302215384</v>
       </c>
       <c r="L23" s="18">
-        <v>0.20206812738172508</v>
+        <v>5.2140192621427994</v>
       </c>
       <c r="M23" s="18">
-        <v>0.16839010615143757</v>
+        <v>4.8432446410198446</v>
       </c>
       <c r="N23" s="18">
-        <v>0.19742288307409922</v>
+        <v>5.4102095818988687</v>
       </c>
       <c r="O23" s="18">
-        <v>0.2</v>
+        <v>5.3645577792123946</v>
       </c>
       <c r="P23" s="18">
-        <v>0.21</v>
+        <v>5.76</v>
       </c>
       <c r="Q23" s="18">
-        <v>0.21</v>
+        <v>5.94</v>
       </c>
       <c r="R23" s="18">
-        <v>0.21</v>
+        <v>6.08</v>
       </c>
       <c r="S23" s="18">
-        <v>0.22</v>
+        <v>6.2</v>
       </c>
       <c r="T23" s="18">
-        <v>0.22</v>
+        <v>6.36</v>
       </c>
       <c r="U23" s="18">
-        <v>0.23</v>
+        <v>6.49</v>
       </c>
       <c r="V23" s="18">
-        <v>0.23</v>
+        <v>6.58</v>
       </c>
       <c r="W23" s="18">
-        <v>0.24</v>
+        <v>6.67</v>
       </c>
       <c r="X23" s="18">
-        <v>0.24</v>
+        <v>6.81</v>
       </c>
       <c r="Y23" s="18">
-        <v>0.24</v>
+        <v>6.9</v>
       </c>
       <c r="Z23" s="18">
-        <v>0.25</v>
+        <v>7.02</v>
       </c>
       <c r="AA23" s="18">
-        <v>0.25</v>
+        <v>7.1</v>
       </c>
       <c r="AB23" s="18">
-        <v>0.26</v>
+        <v>7.19</v>
       </c>
       <c r="AC23" s="18">
-        <v>0.26</v>
+        <v>7.3</v>
       </c>
       <c r="AD23" s="18">
-        <v>0.27</v>
+        <v>7.4</v>
       </c>
       <c r="AE23" s="18">
-        <v>0.27</v>
+        <v>7.51</v>
       </c>
       <c r="AF23" s="18">
-        <v>0.28000000000000003</v>
+        <v>7.65</v>
       </c>
       <c r="AG23" s="18">
-        <v>0.28000000000000003</v>
+        <v>7.78</v>
       </c>
       <c r="AH23" s="18">
-        <v>0.28000000000000003</v>
+        <v>7.93</v>
       </c>
       <c r="AI23" s="18">
-        <v>0.28999999999999998</v>
+        <v>8.08</v>
       </c>
       <c r="AJ23" s="18">
-        <v>0.28999999999999998</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="AK23" s="18">
-        <v>0.3</v>
+        <v>8.4</v>
       </c>
       <c r="AL23" s="18">
-        <v>0.3</v>
+        <v>8.57</v>
       </c>
       <c r="AM23" s="18">
-        <v>0.3</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="AN23" s="18">
-        <v>0.31</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="AO23" s="18">
-        <v>0.31</v>
+        <v>9.16</v>
       </c>
       <c r="AP23" s="18">
-        <v>0.32</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="AQ23" s="18">
-        <v>0.32</v>
+        <v>9.57</v>
       </c>
       <c r="AR23" s="18">
-        <v>0.32</v>
+        <v>9.75</v>
       </c>
       <c r="AS23" s="18">
-        <v>0.33</v>
+        <v>9.94</v>
       </c>
       <c r="AT23" s="18">
-        <v>0.33</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="AU23" s="18">
-        <v>0.34</v>
+        <v>10.33</v>
       </c>
       <c r="AV23" s="18">
-        <v>0.34</v>
+        <v>10.54</v>
       </c>
       <c r="AW23" s="18">
-        <v>0.34</v>
+        <v>10.76</v>
       </c>
       <c r="AX23" s="18">
-        <v>0.35</v>
+        <v>10.98</v>
       </c>
       <c r="AY23" s="18">
-        <v>0.35</v>
+        <v>11.2</v>
       </c>
       <c r="AZ23" s="18">
-        <v>0.35</v>
+        <v>11.44</v>
       </c>
       <c r="BA23" s="18">
-        <v>0.36</v>
+        <v>11.67</v>
       </c>
       <c r="BB23" s="18">
-        <v>0.36</v>
+        <v>11.92</v>
       </c>
       <c r="BC23" s="18">
-        <v>0.36</v>
+        <v>12.16</v>
       </c>
       <c r="BD23" s="18">
-        <v>0.37</v>
+        <v>12.42</v>
       </c>
       <c r="BE23" s="18">
-        <v>0.37</v>
+        <v>12.67</v>
       </c>
       <c r="BF23" s="18">
-        <v>0.37</v>
+        <v>12.93</v>
       </c>
       <c r="BG23" s="18">
-        <v>0.38</v>
+        <v>13.19</v>
       </c>
       <c r="BH23" s="18">
-        <v>0.38</v>
+        <v>13.46</v>
       </c>
       <c r="BI23" s="18">
-        <v>0.38</v>
+        <v>13.73</v>
       </c>
       <c r="BJ23" s="18">
-        <v>0.39</v>
+        <v>14.01</v>
       </c>
       <c r="BK23" s="18">
-        <v>0.39</v>
+        <v>14.3</v>
       </c>
     </row>
-    <row r="24" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>10</v>
       </c>
@@ -3589,7 +3553,7 @@
         <v>1.0966180601025668</v>
       </c>
       <c r="O24" s="22">
-        <v>1.1299999999999999</v>
+        <v>1.0278244028405423</v>
       </c>
       <c r="P24" s="22">
         <v>1.17</v>
@@ -3736,7 +3700,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="25" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>10</v>
       </c>
@@ -3927,7 +3891,7 @@
         <v>3.9848753614033661</v>
       </c>
     </row>
-    <row r="26" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>10</v>
       </c>
@@ -3971,7 +3935,7 @@
         <v>5.4102095818988687</v>
       </c>
       <c r="O26" s="22">
-        <v>5.6</v>
+        <v>5.3645577792123946</v>
       </c>
       <c r="P26" s="22">
         <v>5.76</v>
@@ -4118,7 +4082,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="27" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>10</v>
       </c>
@@ -4162,154 +4126,154 @@
         <v>25.150513992563333</v>
       </c>
       <c r="O27" s="18">
-        <v>25.3154</v>
+        <v>26.593867010974826</v>
       </c>
       <c r="P27" s="18">
-        <v>26.482030000000002</v>
+        <v>26.244130000000002</v>
       </c>
       <c r="Q27" s="18">
-        <v>26.69706</v>
+        <v>26.928867500000003</v>
       </c>
       <c r="R27" s="18">
-        <v>27.839320000000001</v>
+        <v>27.569065000000002</v>
       </c>
       <c r="S27" s="18">
-        <v>27.900559999999999</v>
+        <v>28.211665</v>
       </c>
       <c r="T27" s="18">
-        <v>29.206219999999998</v>
+        <v>28.951492500000001</v>
       </c>
       <c r="U27" s="18">
-        <v>29.49297</v>
+        <v>29.685220000000001</v>
       </c>
       <c r="V27" s="18">
-        <v>30.548719999999999</v>
+        <v>30.3404025</v>
       </c>
       <c r="W27" s="18">
-        <v>30.7712</v>
+        <v>31.055710000000001</v>
       </c>
       <c r="X27" s="18">
-        <v>32.131720000000001</v>
+        <v>31.874875000000003</v>
       </c>
       <c r="Y27" s="18">
-        <v>32.464860000000002</v>
+        <v>32.701459999999997</v>
       </c>
       <c r="Z27" s="18">
-        <v>33.744399999999999</v>
+        <v>33.519705000000002</v>
       </c>
       <c r="AA27" s="18">
-        <v>34.125160000000001</v>
+        <v>34.303307500000003</v>
       </c>
       <c r="AB27" s="18">
-        <v>35.218510000000002</v>
+        <v>35.074262500000003</v>
       </c>
       <c r="AC27" s="18">
-        <v>35.734870000000001</v>
+        <v>35.866017499999998</v>
       </c>
       <c r="AD27" s="18">
-        <v>36.775820000000003</v>
+        <v>36.641942499999999</v>
       </c>
       <c r="AE27" s="18">
-        <v>37.281260000000003</v>
+        <v>37.433554999999998</v>
       </c>
       <c r="AF27" s="18">
-        <v>38.395879999999998</v>
+        <v>38.250982499999999</v>
       </c>
       <c r="AG27" s="18">
-        <v>38.930909999999997</v>
+        <v>39.049639999999997</v>
       </c>
       <c r="AH27" s="18">
-        <v>39.940860000000001</v>
+        <v>39.830224999999999</v>
       </c>
       <c r="AI27" s="18">
-        <v>40.508270000000003</v>
+        <v>40.561500000000002</v>
       </c>
       <c r="AJ27" s="18">
-        <v>41.288600000000002</v>
+        <v>41.242282500000002</v>
       </c>
       <c r="AK27" s="18">
-        <v>41.883659999999999</v>
+        <v>41.936534999999999</v>
       </c>
       <c r="AL27" s="18">
-        <v>42.690219999999997</v>
+        <v>42.657607499999997</v>
       </c>
       <c r="AM27" s="18">
-        <v>43.366329999999998</v>
+        <v>43.394719999999992</v>
       </c>
       <c r="AN27" s="18">
-        <v>44.155999999999999</v>
+        <v>44.084127499999994</v>
       </c>
       <c r="AO27" s="18">
-        <v>44.658180000000002</v>
+        <v>44.726309999999998</v>
       </c>
       <c r="AP27" s="18">
-        <v>45.432879999999997</v>
+        <v>45.374772499999999</v>
       </c>
       <c r="AQ27" s="18">
-        <v>45.975149999999999</v>
+        <v>46.030794999999998</v>
       </c>
       <c r="AR27" s="18">
-        <v>46.74</v>
+        <v>46.718787500000005</v>
       </c>
       <c r="AS27" s="18">
-        <v>47.42</v>
+        <v>47.412500000000001</v>
       </c>
       <c r="AT27" s="18">
-        <v>48.07</v>
+        <v>48.08</v>
       </c>
       <c r="AU27" s="18">
-        <v>48.76</v>
+        <v>48.757499999999993</v>
       </c>
       <c r="AV27" s="18">
-        <v>49.44</v>
+        <v>49.445</v>
       </c>
       <c r="AW27" s="18">
-        <v>50.14</v>
+        <v>50.127499999999998</v>
       </c>
       <c r="AX27" s="18">
-        <v>50.79</v>
+        <v>50.792500000000004</v>
       </c>
       <c r="AY27" s="18">
-        <v>51.45</v>
+        <v>51.445</v>
       </c>
       <c r="AZ27" s="18">
-        <v>52.09</v>
+        <v>52.092500000000001</v>
       </c>
       <c r="BA27" s="18">
-        <v>52.74</v>
+        <v>52.732500000000002</v>
       </c>
       <c r="BB27" s="18">
-        <v>53.36</v>
+        <v>53.362499999999997</v>
       </c>
       <c r="BC27" s="18">
-        <v>53.99</v>
+        <v>53.987499999999997</v>
       </c>
       <c r="BD27" s="18">
-        <v>54.61</v>
+        <v>54.607500000000002</v>
       </c>
       <c r="BE27" s="18">
         <v>55.22</v>
       </c>
       <c r="BF27" s="18">
-        <v>55.83</v>
+        <v>55.825000000000003</v>
       </c>
       <c r="BG27" s="18">
-        <v>56.42</v>
+        <v>56.417500000000004</v>
       </c>
       <c r="BH27" s="18">
-        <v>57</v>
+        <v>56.997500000000002</v>
       </c>
       <c r="BI27" s="18">
-        <v>57.57</v>
+        <v>57.567499999999995</v>
       </c>
       <c r="BJ27" s="18">
-        <v>58.13</v>
+        <v>58.127499999999998</v>
       </c>
       <c r="BK27" s="18">
         <v>58.68</v>
       </c>
     </row>
-    <row r="28" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -4353,25 +4317,25 @@
         <v>0.31491248201071131</v>
       </c>
       <c r="O28" s="22">
-        <v>0.32</v>
+        <v>0.31723692704970952</v>
       </c>
       <c r="P28" s="22">
-        <v>0.33</v>
+        <v>0.32750000000000001</v>
       </c>
       <c r="Q28" s="22">
-        <v>0.33</v>
+        <v>0.33499999999999996</v>
       </c>
       <c r="R28" s="22">
-        <v>0.35</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="S28" s="22">
-        <v>0.35</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="T28" s="22">
-        <v>0.37</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="U28" s="22">
-        <v>0.37</v>
+        <v>0.3725</v>
       </c>
       <c r="V28" s="22">
         <v>0.38</v>
@@ -4383,7 +4347,7 @@
         <v>0.4</v>
       </c>
       <c r="Y28" s="22">
-        <v>0.41</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="Z28" s="22">
         <v>0.42</v>
@@ -4398,7 +4362,7 @@
         <v>0.45</v>
       </c>
       <c r="AD28" s="22">
-        <v>0.46</v>
+        <v>0.45999999999999996</v>
       </c>
       <c r="AE28" s="22">
         <v>0.47</v>
@@ -4416,10 +4380,10 @@
         <v>0.51</v>
       </c>
       <c r="AJ28" s="22">
-        <v>0.52</v>
+        <v>0.51750000000000007</v>
       </c>
       <c r="AK28" s="22">
-        <v>0.52</v>
+        <v>0.52249999999999996</v>
       </c>
       <c r="AL28" s="22">
         <v>0.53</v>
@@ -4434,16 +4398,16 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="AP28" s="22">
-        <v>0.56999999999999995</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="AQ28" s="22">
         <v>0.57999999999999996</v>
       </c>
       <c r="AR28" s="22">
-        <v>0.59</v>
+        <v>0.58749999999999991</v>
       </c>
       <c r="AS28" s="22">
-        <v>0.59</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="AT28" s="22">
         <v>0.6</v>
@@ -4458,10 +4422,10 @@
         <v>0.63</v>
       </c>
       <c r="AX28" s="22">
-        <v>0.64</v>
+        <v>0.63749999999999996</v>
       </c>
       <c r="AY28" s="22">
-        <v>0.64</v>
+        <v>0.64250000000000007</v>
       </c>
       <c r="AZ28" s="22">
         <v>0.65</v>
@@ -4473,10 +4437,10 @@
         <v>0.67</v>
       </c>
       <c r="BC28" s="22">
-        <v>0.68</v>
+        <v>0.67749999999999999</v>
       </c>
       <c r="BD28" s="22">
-        <v>0.68</v>
+        <v>0.68250000000000011</v>
       </c>
       <c r="BE28" s="22">
         <v>0.69</v>
@@ -4485,22 +4449,22 @@
         <v>0.7</v>
       </c>
       <c r="BG28" s="22">
-        <v>0.71</v>
+        <v>0.70750000000000002</v>
       </c>
       <c r="BH28" s="22">
-        <v>0.71</v>
+        <v>0.71249999999999991</v>
       </c>
       <c r="BI28" s="22">
         <v>0.72</v>
       </c>
       <c r="BJ28" s="22">
-        <v>0.73</v>
+        <v>0.72750000000000004</v>
       </c>
       <c r="BK28" s="22">
         <v>0.73</v>
       </c>
     </row>
-    <row r="29" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>10</v>
       </c>
@@ -4544,115 +4508,115 @@
         <v>2.3810967562588741</v>
       </c>
       <c r="O29" s="18">
-        <v>2.4</v>
+        <v>2.6552614590058101</v>
       </c>
       <c r="P29" s="18">
-        <v>2.5099999999999998</v>
+        <v>2.4874999999999998</v>
       </c>
       <c r="Q29" s="18">
-        <v>2.5299999999999998</v>
+        <v>2.5525000000000002</v>
       </c>
       <c r="R29" s="18">
-        <v>2.64</v>
+        <v>2.6124999999999998</v>
       </c>
       <c r="S29" s="18">
-        <v>2.64</v>
+        <v>2.6725000000000003</v>
       </c>
       <c r="T29" s="18">
-        <v>2.77</v>
+        <v>2.7424999999999997</v>
       </c>
       <c r="U29" s="18">
-        <v>2.79</v>
+        <v>2.81</v>
       </c>
       <c r="V29" s="18">
-        <v>2.89</v>
+        <v>2.87</v>
       </c>
       <c r="W29" s="18">
-        <v>2.91</v>
+        <v>2.9375</v>
       </c>
       <c r="X29" s="18">
-        <v>3.04</v>
+        <v>3.0150000000000001</v>
       </c>
       <c r="Y29" s="18">
-        <v>3.07</v>
+        <v>3.0925000000000002</v>
       </c>
       <c r="Z29" s="18">
-        <v>3.19</v>
+        <v>3.17</v>
       </c>
       <c r="AA29" s="18">
-        <v>3.23</v>
+        <v>3.2450000000000001</v>
       </c>
       <c r="AB29" s="18">
-        <v>3.33</v>
+        <v>3.3174999999999999</v>
       </c>
       <c r="AC29" s="18">
-        <v>3.38</v>
+        <v>3.3925000000000001</v>
       </c>
       <c r="AD29" s="18">
-        <v>3.48</v>
+        <v>3.4675000000000002</v>
       </c>
       <c r="AE29" s="18">
-        <v>3.53</v>
+        <v>3.5449999999999999</v>
       </c>
       <c r="AF29" s="18">
-        <v>3.64</v>
+        <v>3.625</v>
       </c>
       <c r="AG29" s="18">
-        <v>3.69</v>
+        <v>3.7</v>
       </c>
       <c r="AH29" s="18">
-        <v>3.78</v>
+        <v>3.7725</v>
       </c>
       <c r="AI29" s="18">
-        <v>3.84</v>
+        <v>3.8424999999999998</v>
       </c>
       <c r="AJ29" s="18">
-        <v>3.91</v>
+        <v>3.9075000000000002</v>
       </c>
       <c r="AK29" s="18">
-        <v>3.97</v>
+        <v>3.9725000000000001</v>
       </c>
       <c r="AL29" s="18">
         <v>4.04</v>
       </c>
       <c r="AM29" s="18">
-        <v>4.1100000000000003</v>
+        <v>4.1099999999999994</v>
       </c>
       <c r="AN29" s="18">
-        <v>4.18</v>
+        <v>4.1749999999999998</v>
       </c>
       <c r="AO29" s="18">
-        <v>4.2300000000000004</v>
+        <v>4.2350000000000003</v>
       </c>
       <c r="AP29" s="18">
-        <v>4.3</v>
+        <v>4.2949999999999999</v>
       </c>
       <c r="AQ29" s="18">
-        <v>4.3499999999999996</v>
+        <v>4.3574999999999999</v>
       </c>
       <c r="AR29" s="18">
-        <v>4.43</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="AS29" s="18">
         <v>4.49</v>
       </c>
       <c r="AT29" s="18">
-        <v>4.55</v>
+        <v>4.5525000000000002</v>
       </c>
       <c r="AU29" s="18">
-        <v>4.62</v>
+        <v>4.6174999999999997</v>
       </c>
       <c r="AV29" s="18">
-        <v>4.68</v>
+        <v>4.6825000000000001</v>
       </c>
       <c r="AW29" s="18">
-        <v>4.75</v>
+        <v>4.7474999999999996</v>
       </c>
       <c r="AX29" s="18">
-        <v>4.8099999999999996</v>
+        <v>4.8100000000000005</v>
       </c>
       <c r="AY29" s="18">
-        <v>4.87</v>
+        <v>4.8699999999999992</v>
       </c>
       <c r="AZ29" s="18">
         <v>4.93</v>
@@ -4661,10 +4625,10 @@
         <v>4.99</v>
       </c>
       <c r="BB29" s="18">
-        <v>5.05</v>
+        <v>5.0500000000000007</v>
       </c>
       <c r="BC29" s="18">
-        <v>5.1100000000000003</v>
+        <v>5.1099999999999994</v>
       </c>
       <c r="BD29" s="18">
         <v>5.17</v>
@@ -4673,25 +4637,25 @@
         <v>5.23</v>
       </c>
       <c r="BF29" s="18">
-        <v>5.29</v>
+        <v>5.2874999999999996</v>
       </c>
       <c r="BG29" s="18">
-        <v>5.34</v>
+        <v>5.3425000000000002</v>
       </c>
       <c r="BH29" s="18">
-        <v>5.4</v>
+        <v>5.3975</v>
       </c>
       <c r="BI29" s="18">
         <v>5.45</v>
       </c>
       <c r="BJ29" s="18">
-        <v>5.5</v>
+        <v>5.5024999999999995</v>
       </c>
       <c r="BK29" s="18">
         <v>5.56</v>
       </c>
     </row>
-    <row r="30" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>10</v>
       </c>
@@ -4735,139 +4699,139 @@
         <v>4.3899411636953181</v>
       </c>
       <c r="O30" s="22">
-        <v>4.42</v>
+        <v>6.0873466752743708</v>
       </c>
       <c r="P30" s="22">
-        <v>4.62</v>
+        <v>4.58</v>
       </c>
       <c r="Q30" s="22">
-        <v>4.66</v>
+        <v>4.7</v>
       </c>
       <c r="R30" s="22">
-        <v>4.8600000000000003</v>
+        <v>4.8125</v>
       </c>
       <c r="S30" s="22">
-        <v>4.87</v>
+        <v>4.9250000000000007</v>
       </c>
       <c r="T30" s="22">
-        <v>5.0999999999999996</v>
+        <v>5.0549999999999997</v>
       </c>
       <c r="U30" s="22">
-        <v>5.15</v>
+        <v>5.1825000000000001</v>
       </c>
       <c r="V30" s="22">
-        <v>5.33</v>
+        <v>5.2949999999999999</v>
       </c>
       <c r="W30" s="22">
-        <v>5.37</v>
+        <v>5.42</v>
       </c>
       <c r="X30" s="22">
-        <v>5.61</v>
+        <v>5.5649999999999995</v>
       </c>
       <c r="Y30" s="22">
-        <v>5.67</v>
+        <v>5.71</v>
       </c>
       <c r="Z30" s="22">
-        <v>5.89</v>
+        <v>5.8524999999999991</v>
       </c>
       <c r="AA30" s="22">
-        <v>5.96</v>
+        <v>5.99</v>
       </c>
       <c r="AB30" s="22">
-        <v>6.15</v>
+        <v>6.125</v>
       </c>
       <c r="AC30" s="22">
-        <v>6.24</v>
+        <v>6.2625000000000002</v>
       </c>
       <c r="AD30" s="22">
-        <v>6.42</v>
+        <v>6.3975</v>
       </c>
       <c r="AE30" s="22">
-        <v>6.51</v>
+        <v>6.5350000000000001</v>
       </c>
       <c r="AF30" s="22">
-        <v>6.7</v>
+        <v>6.6775000000000002</v>
       </c>
       <c r="AG30" s="22">
-        <v>6.8</v>
+        <v>6.8174999999999999</v>
       </c>
       <c r="AH30" s="22">
-        <v>6.97</v>
+        <v>6.9525000000000006</v>
       </c>
       <c r="AI30" s="22">
-        <v>7.07</v>
+        <v>7.08</v>
       </c>
       <c r="AJ30" s="22">
-        <v>7.21</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="AK30" s="22">
-        <v>7.31</v>
+        <v>7.32</v>
       </c>
       <c r="AL30" s="22">
-        <v>7.45</v>
+        <v>7.4450000000000003</v>
       </c>
       <c r="AM30" s="22">
-        <v>7.57</v>
+        <v>7.5750000000000002</v>
       </c>
       <c r="AN30" s="22">
-        <v>7.71</v>
+        <v>7.6950000000000003</v>
       </c>
       <c r="AO30" s="22">
-        <v>7.79</v>
+        <v>7.8049999999999997</v>
       </c>
       <c r="AP30" s="22">
-        <v>7.93</v>
+        <v>7.9174999999999995</v>
       </c>
       <c r="AQ30" s="22">
-        <v>8.02</v>
+        <v>8.0324999999999989</v>
       </c>
       <c r="AR30" s="22">
-        <v>8.16</v>
+        <v>8.1549999999999994</v>
       </c>
       <c r="AS30" s="22">
-        <v>8.2799999999999994</v>
+        <v>8.2774999999999999</v>
       </c>
       <c r="AT30" s="22">
-        <v>8.39</v>
+        <v>8.3925000000000001</v>
       </c>
       <c r="AU30" s="22">
-        <v>8.51</v>
+        <v>8.5100000000000016</v>
       </c>
       <c r="AV30" s="22">
-        <v>8.6300000000000008</v>
+        <v>8.629999999999999</v>
       </c>
       <c r="AW30" s="22">
-        <v>8.75</v>
+        <v>8.7475000000000005</v>
       </c>
       <c r="AX30" s="22">
-        <v>8.86</v>
+        <v>8.8625000000000007</v>
       </c>
       <c r="AY30" s="22">
-        <v>8.98</v>
+        <v>8.9774999999999991</v>
       </c>
       <c r="AZ30" s="22">
-        <v>9.09</v>
+        <v>9.0925000000000011</v>
       </c>
       <c r="BA30" s="22">
-        <v>9.2100000000000009</v>
+        <v>9.2050000000000001</v>
       </c>
       <c r="BB30" s="22">
-        <v>9.31</v>
+        <v>9.3125</v>
       </c>
       <c r="BC30" s="22">
         <v>9.42</v>
       </c>
       <c r="BD30" s="22">
-        <v>9.5299999999999994</v>
+        <v>9.5300000000000011</v>
       </c>
       <c r="BE30" s="22">
-        <v>9.64</v>
+        <v>9.6374999999999993</v>
       </c>
       <c r="BF30" s="22">
-        <v>9.74</v>
+        <v>9.7424999999999997</v>
       </c>
       <c r="BG30" s="22">
-        <v>9.85</v>
+        <v>9.8475000000000001</v>
       </c>
       <c r="BH30" s="22">
         <v>9.9499999999999993</v>
@@ -4876,13 +4840,13 @@
         <v>10.050000000000001</v>
       </c>
       <c r="BJ30" s="22">
-        <v>10.15</v>
+        <v>10.147500000000001</v>
       </c>
       <c r="BK30" s="22">
         <v>10.24</v>
       </c>
     </row>
-    <row r="31" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>10</v>
       </c>
@@ -4926,31 +4890,31 @@
         <v>0.23700357618085477</v>
       </c>
       <c r="O31" s="18">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="P31" s="18">
-        <v>0.25</v>
+        <v>0.2475</v>
       </c>
       <c r="Q31" s="18">
-        <v>0.25</v>
+        <v>0.2525</v>
       </c>
       <c r="R31" s="18">
-        <v>0.26</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S31" s="18">
-        <v>0.26</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="T31" s="18">
-        <v>0.28000000000000003</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="U31" s="18">
-        <v>0.28000000000000003</v>
+        <v>0.28250000000000003</v>
       </c>
       <c r="V31" s="18">
-        <v>0.28999999999999998</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="W31" s="18">
-        <v>0.28999999999999998</v>
+        <v>0.29249999999999998</v>
       </c>
       <c r="X31" s="18">
         <v>0.3</v>
@@ -4959,22 +4923,22 @@
         <v>0.31</v>
       </c>
       <c r="Z31" s="18">
-        <v>0.32</v>
+        <v>0.3175</v>
       </c>
       <c r="AA31" s="18">
-        <v>0.32</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="AB31" s="18">
         <v>0.33</v>
       </c>
       <c r="AC31" s="18">
-        <v>0.34</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="AD31" s="18">
-        <v>0.35</v>
+        <v>0.34749999999999998</v>
       </c>
       <c r="AE31" s="18">
-        <v>0.35</v>
+        <v>0.35249999999999998</v>
       </c>
       <c r="AF31" s="18">
         <v>0.36</v>
@@ -4983,97 +4947,97 @@
         <v>0.37</v>
       </c>
       <c r="AH31" s="18">
-        <v>0.38</v>
+        <v>0.3775</v>
       </c>
       <c r="AI31" s="18">
-        <v>0.38</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="AJ31" s="18">
-        <v>0.39</v>
+        <v>0.38750000000000001</v>
       </c>
       <c r="AK31" s="18">
-        <v>0.39</v>
+        <v>0.39250000000000002</v>
       </c>
       <c r="AL31" s="18">
         <v>0.4</v>
       </c>
       <c r="AM31" s="18">
-        <v>0.41</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="AN31" s="18">
-        <v>0.42</v>
+        <v>0.41749999999999998</v>
       </c>
       <c r="AO31" s="18">
-        <v>0.42</v>
+        <v>0.42249999999999999</v>
       </c>
       <c r="AP31" s="18">
-        <v>0.43</v>
+        <v>0.42749999999999999</v>
       </c>
       <c r="AQ31" s="18">
-        <v>0.43</v>
+        <v>0.4325</v>
       </c>
       <c r="AR31" s="18">
         <v>0.44</v>
       </c>
       <c r="AS31" s="18">
-        <v>0.45</v>
+        <v>0.44750000000000001</v>
       </c>
       <c r="AT31" s="18">
-        <v>0.45</v>
+        <v>0.45250000000000001</v>
       </c>
       <c r="AU31" s="18">
-        <v>0.46</v>
+        <v>0.45999999999999996</v>
       </c>
       <c r="AV31" s="18">
-        <v>0.47</v>
+        <v>0.46749999999999997</v>
       </c>
       <c r="AW31" s="18">
-        <v>0.47</v>
+        <v>0.47249999999999998</v>
       </c>
       <c r="AX31" s="18">
-        <v>0.48</v>
+        <v>0.47749999999999998</v>
       </c>
       <c r="AY31" s="18">
-        <v>0.48</v>
+        <v>0.48249999999999998</v>
       </c>
       <c r="AZ31" s="18">
         <v>0.49</v>
       </c>
       <c r="BA31" s="18">
-        <v>0.5</v>
+        <v>0.4975</v>
       </c>
       <c r="BB31" s="18">
-        <v>0.5</v>
+        <v>0.50249999999999995</v>
       </c>
       <c r="BC31" s="18">
-        <v>0.51</v>
+        <v>0.50750000000000006</v>
       </c>
       <c r="BD31" s="18">
-        <v>0.51</v>
+        <v>0.51249999999999996</v>
       </c>
       <c r="BE31" s="18">
         <v>0.52</v>
       </c>
       <c r="BF31" s="18">
-        <v>0.53</v>
+        <v>0.52750000000000008</v>
       </c>
       <c r="BG31" s="18">
-        <v>0.53</v>
+        <v>0.53249999999999997</v>
       </c>
       <c r="BH31" s="18">
-        <v>0.54</v>
+        <v>0.53750000000000009</v>
       </c>
       <c r="BI31" s="18">
-        <v>0.54</v>
+        <v>0.54249999999999998</v>
       </c>
       <c r="BJ31" s="18">
-        <v>0.55000000000000004</v>
+        <v>0.5475000000000001</v>
       </c>
       <c r="BK31" s="18">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>10</v>
       </c>
@@ -5117,118 +5081,118 @@
         <v>2.2581693890446233</v>
       </c>
       <c r="O32" s="22">
-        <v>2.4573100000000001</v>
+        <v>2.7493867010974822</v>
       </c>
       <c r="P32" s="22">
-        <v>2.3857200000000001</v>
+        <v>2.4674200000000002</v>
       </c>
       <c r="Q32" s="22">
-        <v>2.64093</v>
+        <v>2.5505100000000001</v>
       </c>
       <c r="R32" s="22">
-        <v>2.5344600000000002</v>
+        <v>2.6270500000000001</v>
       </c>
       <c r="S32" s="22">
-        <v>2.7983500000000001</v>
+        <v>2.7078875</v>
       </c>
       <c r="T32" s="22">
-        <v>2.7003900000000001</v>
+        <v>2.7961825</v>
       </c>
       <c r="U32" s="22">
-        <v>2.9855999999999998</v>
+        <v>2.8835999999999999</v>
       </c>
       <c r="V32" s="22">
-        <v>2.8628100000000001</v>
+        <v>2.9595275000000001</v>
       </c>
       <c r="W32" s="22">
-        <v>3.1268899999999999</v>
+        <v>3.0402300000000002</v>
       </c>
       <c r="X32" s="22">
-        <v>3.04433</v>
+        <v>3.1271750000000003</v>
       </c>
       <c r="Y32" s="22">
-        <v>3.2931499999999998</v>
+        <v>3.2146224999999999</v>
       </c>
       <c r="Z32" s="22">
-        <v>3.2278600000000002</v>
+        <v>3.3008500000000001</v>
       </c>
       <c r="AA32" s="22">
-        <v>3.4545300000000001</v>
+        <v>3.3838750000000002</v>
       </c>
       <c r="AB32" s="22">
-        <v>3.3985799999999999</v>
+        <v>3.4663374999999998</v>
       </c>
       <c r="AC32" s="22">
-        <v>3.6136599999999999</v>
+        <v>3.5511599999999999</v>
       </c>
       <c r="AD32" s="22">
-        <v>3.5787399999999998</v>
+        <v>3.635675</v>
       </c>
       <c r="AE32" s="22">
-        <v>3.77156</v>
+        <v>3.7223125000000001</v>
       </c>
       <c r="AF32" s="22">
-        <v>3.7673899999999998</v>
+        <v>3.8129925</v>
       </c>
       <c r="AG32" s="22">
-        <v>3.94563</v>
+        <v>3.9025574999999999</v>
       </c>
       <c r="AH32" s="22">
-        <v>3.9515799999999999</v>
+        <v>3.9917124999999998</v>
       </c>
       <c r="AI32" s="22">
-        <v>4.1180599999999998</v>
+        <v>4.0767299999999995</v>
       </c>
       <c r="AJ32" s="22">
-        <v>4.1192200000000003</v>
+        <v>4.1580025000000003</v>
       </c>
       <c r="AK32" s="22">
-        <v>4.2755099999999997</v>
+        <v>4.2413675</v>
       </c>
       <c r="AL32" s="22">
-        <v>4.2952300000000001</v>
+        <v>4.3287750000000003</v>
       </c>
       <c r="AM32" s="22">
-        <v>4.4491300000000003</v>
+        <v>4.4185499999999998</v>
       </c>
       <c r="AN32" s="22">
-        <v>4.4807100000000002</v>
+        <v>4.5045950000000001</v>
       </c>
       <c r="AO32" s="22">
-        <v>4.6078299999999999</v>
+        <v>4.5864950000000002</v>
       </c>
       <c r="AP32" s="22">
-        <v>4.64961</v>
+        <v>4.6700099999999996</v>
       </c>
       <c r="AQ32" s="22">
-        <v>4.7729900000000001</v>
+        <v>4.7688974999999996</v>
       </c>
       <c r="AR32" s="22">
-        <v>4.88</v>
+        <v>4.8757474999999992</v>
       </c>
       <c r="AS32" s="22">
-        <v>4.97</v>
+        <v>4.9749999999999996</v>
       </c>
       <c r="AT32" s="22">
-        <v>5.08</v>
+        <v>5.0774999999999997</v>
       </c>
       <c r="AU32" s="22">
-        <v>5.18</v>
+        <v>5.1825000000000001</v>
       </c>
       <c r="AV32" s="22">
-        <v>5.29</v>
+        <v>5.2874999999999996</v>
       </c>
       <c r="AW32" s="22">
-        <v>5.39</v>
+        <v>5.3925000000000001</v>
       </c>
       <c r="AX32" s="22">
         <v>5.5</v>
       </c>
       <c r="AY32" s="22">
-        <v>5.61</v>
+        <v>5.6099999999999994</v>
       </c>
       <c r="AZ32" s="22">
-        <v>5.72</v>
+        <v>5.7225000000000001</v>
       </c>
       <c r="BA32" s="22">
         <v>5.84</v>
@@ -5240,7 +5204,7 @@
         <v>6.08</v>
       </c>
       <c r="BD32" s="22">
-        <v>6.2</v>
+        <v>6.2025000000000006</v>
       </c>
       <c r="BE32" s="22">
         <v>6.33</v>
@@ -5252,10 +5216,10 @@
         <v>6.59</v>
       </c>
       <c r="BH32" s="22">
-        <v>6.72</v>
+        <v>6.7225000000000001</v>
       </c>
       <c r="BI32" s="22">
-        <v>6.86</v>
+        <v>6.8599999999999994</v>
       </c>
       <c r="BJ32" s="22">
         <v>7</v>
@@ -5264,7 +5228,7 @@
         <v>7.14</v>
       </c>
     </row>
-    <row r="33" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>10</v>
       </c>
@@ -5308,94 +5272,94 @@
         <v>1.8325867497126211</v>
       </c>
       <c r="O33" s="18">
-        <v>1.99</v>
+        <v>2.4914138153647514</v>
       </c>
       <c r="P33" s="18">
-        <v>1.94</v>
+        <v>2.0024999999999999</v>
       </c>
       <c r="Q33" s="18">
-        <v>2.14</v>
+        <v>2.0700000000000003</v>
       </c>
       <c r="R33" s="18">
-        <v>2.06</v>
+        <v>2.1325000000000003</v>
       </c>
       <c r="S33" s="18">
-        <v>2.27</v>
+        <v>2.1974999999999998</v>
       </c>
       <c r="T33" s="18">
-        <v>2.19</v>
+        <v>2.2675000000000001</v>
       </c>
       <c r="U33" s="18">
-        <v>2.42</v>
+        <v>2.3374999999999999</v>
       </c>
       <c r="V33" s="18">
-        <v>2.3199999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="W33" s="18">
-        <v>2.54</v>
+        <v>2.4675000000000002</v>
       </c>
       <c r="X33" s="18">
-        <v>2.4700000000000002</v>
+        <v>2.5375000000000001</v>
       </c>
       <c r="Y33" s="18">
-        <v>2.67</v>
+        <v>2.6074999999999999</v>
       </c>
       <c r="Z33" s="18">
-        <v>2.62</v>
+        <v>2.6775000000000002</v>
       </c>
       <c r="AA33" s="18">
-        <v>2.8</v>
+        <v>2.7450000000000001</v>
       </c>
       <c r="AB33" s="18">
-        <v>2.76</v>
+        <v>2.8125</v>
       </c>
       <c r="AC33" s="18">
-        <v>2.93</v>
+        <v>2.88</v>
       </c>
       <c r="AD33" s="18">
-        <v>2.9</v>
+        <v>2.9474999999999998</v>
       </c>
       <c r="AE33" s="18">
-        <v>3.06</v>
+        <v>3.02</v>
       </c>
       <c r="AF33" s="18">
-        <v>3.06</v>
+        <v>3.0949999999999998</v>
       </c>
       <c r="AG33" s="18">
-        <v>3.2</v>
+        <v>3.1675</v>
       </c>
       <c r="AH33" s="18">
-        <v>3.21</v>
+        <v>3.24</v>
       </c>
       <c r="AI33" s="18">
-        <v>3.34</v>
+        <v>3.3075000000000001</v>
       </c>
       <c r="AJ33" s="18">
-        <v>3.34</v>
+        <v>3.3725000000000001</v>
       </c>
       <c r="AK33" s="18">
-        <v>3.47</v>
+        <v>3.4424999999999999</v>
       </c>
       <c r="AL33" s="18">
-        <v>3.49</v>
+        <v>3.5150000000000001</v>
       </c>
       <c r="AM33" s="18">
-        <v>3.61</v>
+        <v>3.5875000000000004</v>
       </c>
       <c r="AN33" s="18">
-        <v>3.64</v>
+        <v>3.6574999999999998</v>
       </c>
       <c r="AO33" s="18">
-        <v>3.74</v>
+        <v>3.7225000000000001</v>
       </c>
       <c r="AP33" s="18">
-        <v>3.77</v>
+        <v>3.7875000000000001</v>
       </c>
       <c r="AQ33" s="18">
-        <v>3.87</v>
+        <v>3.8675000000000002</v>
       </c>
       <c r="AR33" s="18">
-        <v>3.96</v>
+        <v>3.9575</v>
       </c>
       <c r="AS33" s="18">
         <v>4.04</v>
@@ -5404,40 +5368,40 @@
         <v>4.12</v>
       </c>
       <c r="AU33" s="18">
-        <v>4.2</v>
+        <v>4.2025000000000006</v>
       </c>
       <c r="AV33" s="18">
-        <v>4.29</v>
+        <v>4.2874999999999996</v>
       </c>
       <c r="AW33" s="18">
-        <v>4.37</v>
+        <v>4.3725000000000005</v>
       </c>
       <c r="AX33" s="18">
         <v>4.46</v>
       </c>
       <c r="AY33" s="18">
-        <v>4.55</v>
+        <v>4.5525000000000002</v>
       </c>
       <c r="AZ33" s="18">
-        <v>4.6500000000000004</v>
+        <v>4.6475</v>
       </c>
       <c r="BA33" s="18">
-        <v>4.74</v>
+        <v>4.7424999999999997</v>
       </c>
       <c r="BB33" s="18">
         <v>4.84</v>
       </c>
       <c r="BC33" s="18">
-        <v>4.9400000000000004</v>
+        <v>4.9399999999999995</v>
       </c>
       <c r="BD33" s="18">
         <v>5.04</v>
       </c>
       <c r="BE33" s="18">
-        <v>5.14</v>
+        <v>5.1400000000000006</v>
       </c>
       <c r="BF33" s="18">
-        <v>5.24</v>
+        <v>5.2424999999999997</v>
       </c>
       <c r="BG33" s="18">
         <v>5.35</v>
@@ -5449,13 +5413,13 @@
         <v>5.57</v>
       </c>
       <c r="BJ33" s="18">
-        <v>5.68</v>
+        <v>5.6825000000000001</v>
       </c>
       <c r="BK33" s="18">
         <v>5.8</v>
       </c>
     </row>
-    <row r="34" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>10</v>
       </c>
@@ -5499,154 +5463,154 @@
         <v>8.6230478354968447</v>
       </c>
       <c r="O34" s="22">
-        <v>9.3800000000000008</v>
+        <v>9.8256294383473204</v>
       </c>
       <c r="P34" s="22">
-        <v>9.11</v>
+        <v>9.42</v>
       </c>
       <c r="Q34" s="22">
-        <v>10.08</v>
+        <v>9.7375000000000007</v>
       </c>
       <c r="R34" s="22">
-        <v>9.68</v>
+        <v>10.032499999999999</v>
       </c>
       <c r="S34" s="22">
-        <v>10.69</v>
+        <v>10.342500000000001</v>
       </c>
       <c r="T34" s="22">
-        <v>10.31</v>
+        <v>10.6775</v>
       </c>
       <c r="U34" s="22">
-        <v>11.4</v>
+        <v>11.010000000000002</v>
       </c>
       <c r="V34" s="22">
-        <v>10.93</v>
+        <v>11.3</v>
       </c>
       <c r="W34" s="22">
-        <v>11.94</v>
+        <v>11.61</v>
       </c>
       <c r="X34" s="22">
-        <v>11.63</v>
+        <v>11.945</v>
       </c>
       <c r="Y34" s="22">
-        <v>12.58</v>
+        <v>12.280000000000001</v>
       </c>
       <c r="Z34" s="22">
-        <v>12.33</v>
+        <v>12.6075</v>
       </c>
       <c r="AA34" s="22">
-        <v>13.19</v>
+        <v>12.922499999999999</v>
       </c>
       <c r="AB34" s="22">
-        <v>12.98</v>
+        <v>13.237500000000001</v>
       </c>
       <c r="AC34" s="22">
-        <v>13.8</v>
+        <v>13.5625</v>
       </c>
       <c r="AD34" s="22">
-        <v>13.67</v>
+        <v>13.885000000000002</v>
       </c>
       <c r="AE34" s="22">
-        <v>14.4</v>
+        <v>14.215</v>
       </c>
       <c r="AF34" s="22">
-        <v>14.39</v>
+        <v>14.5625</v>
       </c>
       <c r="AG34" s="22">
-        <v>15.07</v>
+        <v>14.905000000000001</v>
       </c>
       <c r="AH34" s="22">
-        <v>15.09</v>
+        <v>15.245000000000001</v>
       </c>
       <c r="AI34" s="22">
-        <v>15.73</v>
+        <v>15.57</v>
       </c>
       <c r="AJ34" s="22">
-        <v>15.73</v>
+        <v>15.88</v>
       </c>
       <c r="AK34" s="22">
-        <v>16.329999999999998</v>
+        <v>16.197499999999998</v>
       </c>
       <c r="AL34" s="22">
-        <v>16.399999999999999</v>
+        <v>16.529999999999998</v>
       </c>
       <c r="AM34" s="22">
-        <v>16.989999999999998</v>
+        <v>16.872499999999999</v>
       </c>
       <c r="AN34" s="22">
-        <v>17.11</v>
+        <v>17.202500000000001</v>
       </c>
       <c r="AO34" s="22">
-        <v>17.600000000000001</v>
+        <v>17.515000000000001</v>
       </c>
       <c r="AP34" s="22">
-        <v>17.75</v>
+        <v>17.8325</v>
       </c>
       <c r="AQ34" s="22">
-        <v>18.23</v>
+        <v>18.21</v>
       </c>
       <c r="AR34" s="22">
-        <v>18.63</v>
+        <v>18.619999999999997</v>
       </c>
       <c r="AS34" s="22">
-        <v>18.989999999999998</v>
+        <v>19</v>
       </c>
       <c r="AT34" s="22">
-        <v>19.39</v>
+        <v>19.384999999999998</v>
       </c>
       <c r="AU34" s="22">
-        <v>19.77</v>
+        <v>19.7775</v>
       </c>
       <c r="AV34" s="22">
-        <v>20.18</v>
+        <v>20.177499999999998</v>
       </c>
       <c r="AW34" s="22">
-        <v>20.58</v>
+        <v>20.587499999999999</v>
       </c>
       <c r="AX34" s="22">
-        <v>21.01</v>
+        <v>21.005000000000003</v>
       </c>
       <c r="AY34" s="22">
-        <v>21.42</v>
+        <v>21.427500000000002</v>
       </c>
       <c r="AZ34" s="22">
-        <v>21.86</v>
+        <v>21.857500000000002</v>
       </c>
       <c r="BA34" s="22">
-        <v>22.29</v>
+        <v>22.3</v>
       </c>
       <c r="BB34" s="22">
-        <v>22.76</v>
+        <v>22.7575</v>
       </c>
       <c r="BC34" s="22">
-        <v>23.22</v>
+        <v>23.2225</v>
       </c>
       <c r="BD34" s="22">
-        <v>23.69</v>
+        <v>23.692500000000003</v>
       </c>
       <c r="BE34" s="22">
-        <v>24.17</v>
+        <v>24.172499999999999</v>
       </c>
       <c r="BF34" s="22">
-        <v>24.66</v>
+        <v>24.662500000000001</v>
       </c>
       <c r="BG34" s="22">
-        <v>25.16</v>
+        <v>25.162500000000001</v>
       </c>
       <c r="BH34" s="22">
-        <v>25.67</v>
+        <v>25.675000000000001</v>
       </c>
       <c r="BI34" s="22">
-        <v>26.2</v>
+        <v>26.200000000000003</v>
       </c>
       <c r="BJ34" s="22">
-        <v>26.73</v>
+        <v>26.732500000000002</v>
       </c>
       <c r="BK34" s="22">
         <v>27.27</v>
       </c>
     </row>
-    <row r="35" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>10</v>
       </c>
@@ -5837,7 +5801,7 @@
         <v>3.9848753614033661</v>
       </c>
     </row>
-    <row r="36" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>10</v>
       </c>
@@ -5881,121 +5845,121 @@
         <v>3.1559712018167967</v>
       </c>
       <c r="O36" s="22">
-        <v>3.43</v>
+        <v>5.8671400903808903</v>
       </c>
       <c r="P36" s="22">
-        <v>3.33</v>
+        <v>3.4450000000000003</v>
       </c>
       <c r="Q36" s="22">
-        <v>3.69</v>
+        <v>3.5625</v>
       </c>
       <c r="R36" s="22">
-        <v>3.54</v>
+        <v>3.67</v>
       </c>
       <c r="S36" s="22">
-        <v>3.91</v>
+        <v>3.7825000000000002</v>
       </c>
       <c r="T36" s="22">
-        <v>3.77</v>
+        <v>3.9050000000000002</v>
       </c>
       <c r="U36" s="22">
-        <v>4.17</v>
+        <v>4.0274999999999999</v>
       </c>
       <c r="V36" s="22">
-        <v>4</v>
+        <v>4.1349999999999998</v>
       </c>
       <c r="W36" s="22">
-        <v>4.37</v>
+        <v>4.2475000000000005</v>
       </c>
       <c r="X36" s="22">
-        <v>4.25</v>
+        <v>4.3674999999999997</v>
       </c>
       <c r="Y36" s="22">
-        <v>4.5999999999999996</v>
+        <v>4.49</v>
       </c>
       <c r="Z36" s="22">
-        <v>4.51</v>
+        <v>4.6124999999999998</v>
       </c>
       <c r="AA36" s="22">
-        <v>4.83</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="AB36" s="22">
-        <v>4.75</v>
+        <v>4.8449999999999998</v>
       </c>
       <c r="AC36" s="22">
-        <v>5.05</v>
+        <v>4.9625000000000004</v>
       </c>
       <c r="AD36" s="22">
-        <v>5</v>
+        <v>5.08</v>
       </c>
       <c r="AE36" s="22">
-        <v>5.27</v>
+        <v>5.2024999999999997</v>
       </c>
       <c r="AF36" s="22">
-        <v>5.27</v>
+        <v>5.33</v>
       </c>
       <c r="AG36" s="22">
-        <v>5.51</v>
+        <v>5.4524999999999997</v>
       </c>
       <c r="AH36" s="22">
-        <v>5.52</v>
+        <v>5.5774999999999997</v>
       </c>
       <c r="AI36" s="22">
-        <v>5.76</v>
+        <v>5.6999999999999993</v>
       </c>
       <c r="AJ36" s="22">
-        <v>5.76</v>
+        <v>5.8149999999999995</v>
       </c>
       <c r="AK36" s="22">
-        <v>5.98</v>
+        <v>5.93</v>
       </c>
       <c r="AL36" s="22">
-        <v>6</v>
+        <v>6.05</v>
       </c>
       <c r="AM36" s="22">
-        <v>6.22</v>
+        <v>6.1749999999999998</v>
       </c>
       <c r="AN36" s="22">
-        <v>6.26</v>
+        <v>6.2949999999999999</v>
       </c>
       <c r="AO36" s="22">
-        <v>6.44</v>
+        <v>6.41</v>
       </c>
       <c r="AP36" s="22">
-        <v>6.5</v>
+        <v>6.5274999999999999</v>
       </c>
       <c r="AQ36" s="22">
-        <v>6.67</v>
+        <v>6.665</v>
       </c>
       <c r="AR36" s="22">
-        <v>6.82</v>
+        <v>6.8150000000000004</v>
       </c>
       <c r="AS36" s="22">
-        <v>6.95</v>
+        <v>6.9550000000000001</v>
       </c>
       <c r="AT36" s="22">
-        <v>7.1</v>
+        <v>7.0949999999999998</v>
       </c>
       <c r="AU36" s="22">
-        <v>7.23</v>
+        <v>7.2374999999999998</v>
       </c>
       <c r="AV36" s="22">
-        <v>7.39</v>
+        <v>7.3849999999999998</v>
       </c>
       <c r="AW36" s="22">
-        <v>7.53</v>
+        <v>7.5350000000000001</v>
       </c>
       <c r="AX36" s="22">
-        <v>7.69</v>
+        <v>7.6875</v>
       </c>
       <c r="AY36" s="22">
-        <v>7.84</v>
+        <v>7.8425000000000002</v>
       </c>
       <c r="AZ36" s="22">
         <v>8</v>
       </c>
       <c r="BA36" s="22">
-        <v>8.16</v>
+        <v>8.1624999999999996</v>
       </c>
       <c r="BB36" s="22">
         <v>8.33</v>
@@ -6004,16 +5968,16 @@
         <v>8.5</v>
       </c>
       <c r="BD36" s="22">
-        <v>8.67</v>
+        <v>8.6724999999999994</v>
       </c>
       <c r="BE36" s="22">
         <v>8.85</v>
       </c>
       <c r="BF36" s="22">
-        <v>9.0299999999999994</v>
+        <v>9.0300000000000011</v>
       </c>
       <c r="BG36" s="22">
-        <v>9.2100000000000009</v>
+        <v>9.2125000000000004</v>
       </c>
       <c r="BH36" s="22">
         <v>9.4</v>
@@ -6022,13 +5986,13 @@
         <v>9.59</v>
       </c>
       <c r="BJ36" s="22">
-        <v>9.7799999999999994</v>
+        <v>9.7824999999999989</v>
       </c>
       <c r="BK36" s="22">
         <v>9.98</v>
       </c>
     </row>
-    <row r="37" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>10</v>
       </c>
@@ -6072,162 +6036,162 @@
         <v>20.302984914974349</v>
       </c>
       <c r="O37" s="18">
-        <v>22.09</v>
+        <v>17.793156875403486</v>
       </c>
       <c r="P37" s="18">
-        <v>21.45</v>
+        <v>22.182499999999997</v>
       </c>
       <c r="Q37" s="18">
-        <v>23.74</v>
+        <v>22.93</v>
       </c>
       <c r="R37" s="18">
-        <v>22.79</v>
+        <v>23.619999999999997</v>
       </c>
       <c r="S37" s="18">
-        <v>25.16</v>
+        <v>24.3475</v>
       </c>
       <c r="T37" s="18">
-        <v>24.28</v>
+        <v>25.14</v>
       </c>
       <c r="U37" s="18">
-        <v>26.84</v>
+        <v>25.924999999999997</v>
       </c>
       <c r="V37" s="18">
-        <v>25.74</v>
+        <v>26.607500000000002</v>
       </c>
       <c r="W37" s="18">
-        <v>28.11</v>
+        <v>27.3325</v>
       </c>
       <c r="X37" s="18">
-        <v>27.37</v>
+        <v>28.115000000000002</v>
       </c>
       <c r="Y37" s="18">
-        <v>29.61</v>
+        <v>28.9025</v>
       </c>
       <c r="Z37" s="18">
-        <v>29.02</v>
+        <v>29.677500000000002</v>
       </c>
       <c r="AA37" s="18">
-        <v>31.06</v>
+        <v>30.424999999999997</v>
       </c>
       <c r="AB37" s="18">
-        <v>30.56</v>
+        <v>31.167499999999997</v>
       </c>
       <c r="AC37" s="18">
-        <v>32.49</v>
+        <v>31.93</v>
       </c>
       <c r="AD37" s="18">
-        <v>32.18</v>
+        <v>32.69</v>
       </c>
       <c r="AE37" s="18">
-        <v>33.909999999999997</v>
+        <v>33.467500000000001</v>
       </c>
       <c r="AF37" s="18">
-        <v>33.869999999999997</v>
+        <v>34.28</v>
       </c>
       <c r="AG37" s="18">
-        <v>35.47</v>
+        <v>35.085000000000001</v>
       </c>
       <c r="AH37" s="18">
-        <v>35.53</v>
+        <v>35.89</v>
       </c>
       <c r="AI37" s="18">
-        <v>37.03</v>
+        <v>36.657499999999999</v>
       </c>
       <c r="AJ37" s="18">
-        <v>37.04</v>
+        <v>37.387500000000003</v>
       </c>
       <c r="AK37" s="18">
-        <v>38.44</v>
+        <v>38.134999999999998</v>
       </c>
       <c r="AL37" s="18">
-        <v>38.619999999999997</v>
+        <v>38.92</v>
       </c>
       <c r="AM37" s="18">
-        <v>40</v>
+        <v>39.727499999999999</v>
       </c>
       <c r="AN37" s="18">
-        <v>40.29</v>
+        <v>40.502499999999998</v>
       </c>
       <c r="AO37" s="18">
-        <v>41.43</v>
+        <v>41.237499999999997</v>
       </c>
       <c r="AP37" s="18">
-        <v>41.8</v>
+        <v>41.984999999999999</v>
       </c>
       <c r="AQ37" s="18">
-        <v>42.91</v>
+        <v>42.8675</v>
       </c>
       <c r="AR37" s="18">
-        <v>43.85</v>
+        <v>43.83</v>
       </c>
       <c r="AS37" s="18">
-        <v>44.71</v>
+        <v>44.732500000000002</v>
       </c>
       <c r="AT37" s="18">
-        <v>45.66</v>
+        <v>45.642499999999998</v>
       </c>
       <c r="AU37" s="18">
-        <v>46.54</v>
+        <v>46.564999999999998</v>
       </c>
       <c r="AV37" s="18">
-        <v>47.52</v>
+        <v>47.507500000000007</v>
       </c>
       <c r="AW37" s="18">
-        <v>48.45</v>
+        <v>48.47</v>
       </c>
       <c r="AX37" s="18">
-        <v>49.46</v>
+        <v>49.447500000000005</v>
       </c>
       <c r="AY37" s="18">
-        <v>50.42</v>
+        <v>50.44</v>
       </c>
       <c r="AZ37" s="18">
-        <v>51.46</v>
+        <v>51.457499999999996</v>
       </c>
       <c r="BA37" s="18">
-        <v>52.49</v>
+        <v>52.504999999999995</v>
       </c>
       <c r="BB37" s="18">
-        <v>53.58</v>
+        <v>53.582499999999996</v>
       </c>
       <c r="BC37" s="18">
-        <v>54.68</v>
+        <v>54.682500000000005</v>
       </c>
       <c r="BD37" s="18">
-        <v>55.79</v>
+        <v>55.795000000000002</v>
       </c>
       <c r="BE37" s="18">
-        <v>56.92</v>
+        <v>56.924999999999997</v>
       </c>
       <c r="BF37" s="18">
-        <v>58.07</v>
+        <v>58.077500000000001</v>
       </c>
       <c r="BG37" s="18">
-        <v>59.25</v>
+        <v>59.255000000000003</v>
       </c>
       <c r="BH37" s="18">
-        <v>60.45</v>
+        <v>60.457500000000003</v>
       </c>
       <c r="BI37" s="18">
-        <v>61.68</v>
+        <v>61.685000000000002</v>
       </c>
       <c r="BJ37" s="18">
-        <v>62.93</v>
+        <v>62.9375</v>
       </c>
       <c r="BK37" s="18">
         <v>64.209999999999994</v>
       </c>
     </row>
-    <row r="38" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B38" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>157</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>158</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>13</v>
@@ -6410,15 +6374,15 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="39" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>13</v>
@@ -6601,15 +6565,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>13</v>
@@ -6792,15 +6756,15 @@
         <v>2.2416534877663339</v>
       </c>
     </row>
-    <row r="41" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>13</v>
@@ -6983,15 +6947,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>13</v>
@@ -7174,7 +7138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>10</v>
       </c>
@@ -7365,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>10</v>
       </c>
@@ -7556,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>10</v>
       </c>
@@ -7600,154 +7564,154 @@
         <v>1.8856843657413787</v>
       </c>
       <c r="O45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="P45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="Q45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="R45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="S45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="T45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="U45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="V45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="W45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="X45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="Y45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="Z45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AA45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AB45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AC45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AD45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AE45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AF45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AG45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AH45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AI45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AJ45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AK45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AL45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AM45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AN45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AO45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AP45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AQ45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AR45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AS45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AT45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AU45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AV45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AW45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AX45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AY45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="AZ45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BA45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BB45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BC45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BD45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BE45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BF45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BG45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BH45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BI45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BJ45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
       <c r="BK45" s="18">
-        <v>0.91979999999999995</v>
+        <v>3.55</v>
       </c>
     </row>
-    <row r="46" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>10</v>
       </c>
@@ -7938,7 +7902,7 @@
         <v>91.26</v>
       </c>
     </row>
-    <row r="47" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>10</v>
       </c>
@@ -8129,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>10</v>
       </c>
@@ -8320,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>10</v>
       </c>
@@ -8511,7 +8475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>10</v>
       </c>
@@ -8702,7 +8666,7 @@
         <v>34.930799999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>10</v>
       </c>
@@ -8893,7 +8857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>10</v>
       </c>
@@ -8937,7 +8901,7 @@
         <v>40.945505949568179</v>
       </c>
       <c r="O52" s="22">
-        <v>42.492939999999997</v>
+        <v>42.48766946417043</v>
       </c>
       <c r="P52" s="22">
         <v>43.412210000000002</v>
@@ -9084,7 +9048,7 @@
         <v>115.41</v>
       </c>
     </row>
-    <row r="53" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>10</v>
       </c>
@@ -9128,7 +9092,7 @@
         <v>2.1627173296284621</v>
       </c>
       <c r="O53" s="18">
-        <v>2.2400000000000002</v>
+        <v>2.2072950290510005</v>
       </c>
       <c r="P53" s="18">
         <v>2.29</v>
@@ -9275,7 +9239,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="54" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>10</v>
       </c>
@@ -9319,7 +9283,7 @@
         <v>10.852196815581776</v>
       </c>
       <c r="O54" s="22">
-        <v>11.26</v>
+        <v>10.928405422853453</v>
       </c>
       <c r="P54" s="22">
         <v>11.51</v>
@@ -9466,7 +9430,7 @@
         <v>30.59</v>
       </c>
     </row>
-    <row r="55" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>10</v>
       </c>
@@ -9657,7 +9621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>10</v>
       </c>
@@ -9848,7 +9812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>10</v>
       </c>
@@ -9892,7 +9856,7 @@
         <v>4.1259797721260085</v>
       </c>
       <c r="O57" s="18">
-        <v>4.28</v>
+        <v>4.250161394448031</v>
       </c>
       <c r="P57" s="18">
         <v>4.37</v>
@@ -10039,7 +10003,7 @@
         <v>11.63</v>
       </c>
     </row>
-    <row r="58" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>10</v>
       </c>
@@ -10083,7 +10047,7 @@
         <v>1.6548595399193049</v>
       </c>
       <c r="O58" s="22">
-        <v>1.72</v>
+        <v>1.7430600387346675</v>
       </c>
       <c r="P58" s="22">
         <v>1.75</v>
@@ -10230,7 +10194,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="59" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>10</v>
       </c>
@@ -10274,7 +10238,7 @@
         <v>20.510462487417858</v>
       </c>
       <c r="O59" s="18">
-        <v>21.29</v>
+        <v>28.440348612007746</v>
       </c>
       <c r="P59" s="18">
         <v>21.75</v>
@@ -10421,7 +10385,7 @@
         <v>57.81</v>
       </c>
     </row>
-    <row r="60" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
         <v>10</v>
       </c>
@@ -10465,7 +10429,7 @@
         <v>1.0382512099048955</v>
       </c>
       <c r="O60" s="22">
-        <v>1.08</v>
+        <v>0.90639122014202711</v>
       </c>
       <c r="P60" s="22">
         <v>1.1000000000000001</v>
@@ -10612,7 +10576,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="61" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>10</v>
       </c>
@@ -10656,7 +10620,7 @@
         <v>7.6698878333929388</v>
       </c>
       <c r="O61" s="18">
-        <v>7.67</v>
+        <v>5.5353776630083926</v>
       </c>
       <c r="P61" s="18">
         <v>7.67</v>
@@ -10803,7 +10767,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="62" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>10</v>
       </c>
@@ -10994,7 +10958,7 @@
         <v>1.5084116925338837</v>
       </c>
     </row>
-    <row r="63" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>10</v>
       </c>
@@ -11038,7 +11002,7 @@
         <v>28.635027878821187</v>
       </c>
       <c r="O63" s="18">
-        <v>29.01998</v>
+        <v>28.19864428663654</v>
       </c>
       <c r="P63" s="18">
         <v>29.40164</v>
@@ -11185,7 +11149,7 @@
         <v>40.369999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
         <v>10</v>
       </c>
@@ -11229,7 +11193,7 @@
         <v>7.1160819999999996</v>
       </c>
       <c r="O64" s="22">
-        <v>6.8927149999999999</v>
+        <v>6.5004519044544864</v>
       </c>
       <c r="P64" s="22">
         <v>6.6692999999999998</v>
@@ -11376,7 +11340,7 @@
         <v>3.5620949999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>10</v>
       </c>
@@ -11420,7 +11384,7 @@
         <v>39.917656399749696</v>
       </c>
       <c r="O65" s="18">
-        <v>40.450000000000003</v>
+        <v>41.302969657843768</v>
       </c>
       <c r="P65" s="18">
         <v>40.99</v>
@@ -11567,7 +11531,7 @@
         <v>56.27</v>
       </c>
     </row>
-    <row r="66" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>10</v>
       </c>
@@ -11611,7 +11575,7 @@
         <v>2.3492363900933837E-2</v>
       </c>
       <c r="O66" s="22">
-        <v>0.02</v>
+        <v>3.5442220787604901E-2</v>
       </c>
       <c r="P66" s="22">
         <v>0.02</v>
@@ -11758,7 +11722,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>10</v>
       </c>
@@ -11949,7 +11913,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="68" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
         <v>10</v>
       </c>
@@ -12140,7 +12104,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="69" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:63" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>10</v>
       </c>
@@ -12331,15 +12295,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="70" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:63" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B70" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="C70" s="22" t="s">
-        <v>160</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>13</v>
@@ -12523,6 +12487,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BK70" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12532,24 +12497,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C6432-74C8-462A-9937-6316902B2E10}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
-    <col min="11" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -12575,7 +12540,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
@@ -12613,7 +12578,7 @@
         <v>66.709248950000003</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -12658,7 +12623,7 @@
         <v>0.28162031945646721</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -12703,7 +12668,7 @@
         <v>0.5885997911538472</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -12748,7 +12713,7 @@
         <v>0.1297798893896856</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -12784,7 +12749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>111</v>
       </c>
@@ -12822,7 +12787,7 @@
         <v>31.572428299999999</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>150</v>
       </c>
@@ -12867,7 +12832,7 @@
         <v>0.13160959811254053</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -12912,7 +12877,7 @@
         <v>0.44838340166568685</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>150</v>
       </c>
@@ -12957,7 +12922,7 @@
         <v>0.27768680687763259</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>150</v>
       </c>
@@ -13002,7 +12967,7 @@
         <v>0.14232019334414009</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>122</v>
       </c>
@@ -13040,7 +13005,7 @@
         <v>27.094080000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>150</v>
       </c>
@@ -13082,7 +13047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>137</v>
       </c>
@@ -13117,7 +13082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C17" s="11" t="s">
         <v>139</v>
       </c>
@@ -13144,7 +13109,7 @@
       </c>
       <c r="M17" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>127</v>
       </c>
@@ -13182,7 +13147,7 @@
         <v>9.2856400000000008</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -13224,7 +13189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>132</v>
       </c>
@@ -13262,7 +13227,7 @@
         <v>8.0975474999999992</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>150</v>
       </c>

</xml_diff>